<commit_message>
Final Project Stub - not tested
</commit_message>
<xml_diff>
--- a/SammyShuck_FinalProject/OpenGL_FinalProject_Coordinates.xlsx
+++ b/SammyShuck_FinalProject/OpenGL_FinalProject_Coordinates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sammy\Google Drive\_SNHU_Course_Work\BSCS-Computer_Science\CS-330-J2956_Computer_Graphic_and_Visualization\code\cs330\SammyShuck_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B4BC0D-3980-4365-B2C7-4D2B2058B8FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAB3A1F-121A-4268-9E04-C8767DCD73A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17145" yWindow="2040" windowWidth="16035" windowHeight="10035" xr2:uid="{B5903B6B-09BC-4EBB-A095-2064D8D8038A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="84">
   <si>
     <t>table top</t>
   </si>
@@ -268,6 +268,24 @@
   </si>
   <si>
     <t>0.4610f,0.2110f,-0.5000f</t>
+  </si>
+  <si>
+    <t>0,1,3  2,3,0</t>
+  </si>
+  <si>
+    <t>4,5,7  6,7,4</t>
+  </si>
+  <si>
+    <t>4,5,1  0,1,4</t>
+  </si>
+  <si>
+    <t>2,3 7  6,7,2</t>
+  </si>
+  <si>
+    <t>4,0,2   6,2,4</t>
+  </si>
+  <si>
+    <t>5,1,3  7,3,5</t>
   </si>
 </sst>
 </file>
@@ -832,7 +850,7 @@
   <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D8" sqref="C6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,19 +858,20 @@
     <col min="1" max="1" width="0.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="25" style="16" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="2"/>
+    <col min="5" max="5" width="11.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
     <col min="7" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -862,8 +881,11 @@
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="10" t="s">
         <v>19</v>
@@ -872,7 +894,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
@@ -882,8 +904,11 @@
       <c r="D5" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
         <v>19</v>
@@ -892,7 +917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
@@ -902,8 +927,11 @@
       <c r="D7" s="17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -912,7 +940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>4</v>
       </c>
@@ -922,8 +950,11 @@
       <c r="D9" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="20" t="s">
         <v>20</v>
@@ -932,7 +963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
@@ -942,8 +973,11 @@
       <c r="D11" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
         <v>16</v>
@@ -952,7 +986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
@@ -962,8 +996,11 @@
       <c r="D13" s="14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="21" t="s">
         <v>19</v>
@@ -972,12 +1009,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Working Final Project for Assignment 5-2 Milestone
</commit_message>
<xml_diff>
--- a/SammyShuck_FinalProject/OpenGL_FinalProject_Coordinates.xlsx
+++ b/SammyShuck_FinalProject/OpenGL_FinalProject_Coordinates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sammy\Google Drive\_SNHU_Course_Work\BSCS-Computer_Science\CS-330-J2956_Computer_Graphic_and_Visualization\code\cs330\SammyShuck_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EB0977-1412-493B-BD0C-2F219B190235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D901BF2-C7D6-45F9-A465-FA83F9965146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4485" yWindow="2790" windowWidth="16035" windowHeight="10035" xr2:uid="{B5903B6B-09BC-4EBB-A095-2064D8D8038A}"/>
+    <workbookView xWindow="6525" yWindow="2145" windowWidth="16035" windowHeight="10035" xr2:uid="{B5903B6B-09BC-4EBB-A095-2064D8D8038A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="85">
   <si>
     <t>table top</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>5,1,3  7,3,5</t>
+  </si>
+  <si>
+    <t>-0.500f,0.250f,-0.013f</t>
   </si>
 </sst>
 </file>
@@ -850,7 +853,7 @@
   <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +914,7 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>29</v>
@@ -934,7 +937,7 @@
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>19</v>
@@ -991,7 +994,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>29</v>

</xml_diff>